<commit_message>
Make Mail Service Functionality
</commit_message>
<xml_diff>
--- a/MVCWithBlazor/wwwroot/Fisiere/Prognoza energie zilnic.xlsx
+++ b/MVCWithBlazor/wwwroot/Fisiere/Prognoza energie zilnic.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="07.09.2020" sheetId="1" r:id="rId1"/>
+    <sheet name="05.08.2020" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -120,12 +120,12 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'07.09.2020'!$C$5:$Z$5</c:f>
+              <c:f>'05.08.2020'!$C$5:$Z$5</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'07.09.2020'!$C$6:$Z$6</c:f>
+              <c:f>'05.08.2020'!$C$6:$Z$6</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -142,12 +142,12 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'07.09.2020'!$C$5:$Z$5</c:f>
+              <c:f>'05.08.2020'!$C$5:$Z$5</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'07.09.2020'!$C$7:$Z$7</c:f>
+              <c:f>'05.08.2020'!$C$7:$Z$7</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -379,10 +379,154 @@
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="F6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="I6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="J6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="K6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="L6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="M6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="N6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="O6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="P6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="R6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="S6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="T6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="U6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="V6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="W6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="X6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="Y6" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="Z6" s="0">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="C7" s="0">
+        <v>2.312</v>
+      </c>
+      <c r="D7" s="0">
+        <v>2.296</v>
+      </c>
+      <c r="E7" s="0">
+        <v>2.295</v>
+      </c>
+      <c r="F7" s="0">
+        <v>2.29</v>
+      </c>
+      <c r="G7" s="0">
+        <v>2.287</v>
+      </c>
+      <c r="H7" s="0">
+        <v>2.248</v>
+      </c>
+      <c r="I7" s="0">
+        <v>2.341</v>
+      </c>
+      <c r="J7" s="0">
+        <v>2.383</v>
+      </c>
+      <c r="K7" s="0">
+        <v>1.534</v>
+      </c>
+      <c r="L7" s="0">
+        <v>0.918</v>
+      </c>
+      <c r="M7" s="0">
+        <v>2.171</v>
+      </c>
+      <c r="N7" s="0">
+        <v>2.42</v>
+      </c>
+      <c r="O7" s="0">
+        <v>2.438</v>
+      </c>
+      <c r="P7" s="0">
+        <v>2.393</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>2.344</v>
+      </c>
+      <c r="R7" s="0">
+        <v>2.442</v>
+      </c>
+      <c r="S7" s="0">
+        <v>2.479</v>
+      </c>
+      <c r="T7" s="0">
+        <v>2.41</v>
+      </c>
+      <c r="U7" s="0">
+        <v>2.353</v>
+      </c>
+      <c r="V7" s="0">
+        <v>2.45</v>
+      </c>
+      <c r="W7" s="0">
+        <v>2.499</v>
+      </c>
+      <c r="X7" s="0">
+        <v>2.31</v>
+      </c>
+      <c r="Y7" s="0">
+        <v>2.244</v>
+      </c>
+      <c r="Z7" s="0">
+        <v>2.238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Bug for Daily Consumtion Chart
</commit_message>
<xml_diff>
--- a/MVCWithBlazor/wwwroot/Fisiere/Prognoza energie zilnic.xlsx
+++ b/MVCWithBlazor/wwwroot/Fisiere/Prognoza energie zilnic.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="05.08.2020" sheetId="1" r:id="rId1"/>
+    <sheet name="11.09.2020" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -120,12 +120,12 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05.08.2020'!$C$5:$Z$5</c:f>
+              <c:f>'11.09.2020'!$C$5:$Z$5</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05.08.2020'!$C$6:$Z$6</c:f>
+              <c:f>'11.09.2020'!$C$6:$Z$6</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -142,12 +142,12 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'05.08.2020'!$C$5:$Z$5</c:f>
+              <c:f>'11.09.2020'!$C$5:$Z$5</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05.08.2020'!$C$7:$Z$7</c:f>
+              <c:f>'11.09.2020'!$C$7:$Z$7</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -238,8 +238,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -271,7 +271,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.65765380859375" customWidth="1"/>
+    <col min="2" max="2" width="23.868982315063477" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
@@ -380,76 +380,76 @@
         <v>1</v>
       </c>
       <c r="C6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="H6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="I6" s="0">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="J6" s="0">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="K6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="L6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="M6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="N6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="O6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="P6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="R6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="S6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="T6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="U6" s="0">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="V6" s="0">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="W6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="X6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="Y6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="Z6" s="0">
-        <v>2.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -457,76 +457,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="0">
-        <v>2.312</v>
-      </c>
-      <c r="D7" s="0">
-        <v>2.296</v>
-      </c>
-      <c r="E7" s="0">
-        <v>2.295</v>
-      </c>
-      <c r="F7" s="0">
-        <v>2.29</v>
-      </c>
-      <c r="G7" s="0">
-        <v>2.287</v>
-      </c>
-      <c r="H7" s="0">
-        <v>2.248</v>
-      </c>
-      <c r="I7" s="0">
-        <v>2.341</v>
-      </c>
-      <c r="J7" s="0">
-        <v>2.383</v>
-      </c>
-      <c r="K7" s="0">
-        <v>1.534</v>
-      </c>
-      <c r="L7" s="0">
-        <v>0.918</v>
-      </c>
-      <c r="M7" s="0">
-        <v>2.171</v>
-      </c>
-      <c r="N7" s="0">
-        <v>2.42</v>
-      </c>
-      <c r="O7" s="0">
-        <v>2.438</v>
-      </c>
-      <c r="P7" s="0">
-        <v>2.393</v>
-      </c>
-      <c r="Q7" s="0">
-        <v>2.344</v>
-      </c>
-      <c r="R7" s="0">
-        <v>2.442</v>
-      </c>
-      <c r="S7" s="0">
-        <v>2.479</v>
-      </c>
-      <c r="T7" s="0">
-        <v>2.41</v>
-      </c>
-      <c r="U7" s="0">
-        <v>2.353</v>
-      </c>
-      <c r="V7" s="0">
-        <v>2.45</v>
-      </c>
-      <c r="W7" s="0">
-        <v>2.499</v>
-      </c>
-      <c r="X7" s="0">
-        <v>2.31</v>
-      </c>
-      <c r="Y7" s="0">
-        <v>2.244</v>
-      </c>
-      <c r="Z7" s="0">
-        <v>2.238</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>